<commit_message>
Assume First Nations consume all available water in Law of River
</commit_message>
<xml_diff>
--- a/ModelMusings/PilotFlexAccounting-CombinedPowellMead.xlsx
+++ b/ModelMusings/PilotFlexAccounting-CombinedPowellMead.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\ModelMusings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB661E2D-EDF3-4FBD-AB62-5F936BAC4CDE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6758ECBF-9A0A-4B92-A0EC-ECD66D3DB25A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6645" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6645" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="368">
   <si>
     <t>Year 1</t>
   </si>
@@ -1328,6 +1328,15 @@
   <si>
     <t>MandatoryConservation</t>
   </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>5.0.1</t>
+  </si>
+  <si>
+    <t>In Law of River workbook, assume First Nations consume all available water</t>
+  </si>
 </sst>
 </file>
 
@@ -1827,7 +1836,7 @@
     <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="237">
+  <cellXfs count="240">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2318,6 +2327,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="17" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2361,30 +2394,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="17" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2472,6 +2481,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="13" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -26589,7 +26607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{447CC9A2-4C52-453A-A3CD-EA6E59E26162}">
   <dimension ref="A1:R43"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A37" sqref="A37:L37"/>
     </sheetView>
   </sheetViews>
@@ -26609,20 +26627,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="207" t="s">
+      <c r="A1" s="192" t="s">
         <v>355</v>
       </c>
-      <c r="B1" s="207"/>
-      <c r="C1" s="207"/>
-      <c r="D1" s="207"/>
-      <c r="E1" s="207"/>
-      <c r="F1" s="207"/>
-      <c r="G1" s="207"/>
-      <c r="H1" s="207"/>
-      <c r="I1" s="207"/>
-      <c r="J1" s="207"/>
-      <c r="K1" s="207"/>
-      <c r="L1" s="207"/>
+      <c r="B1" s="192"/>
+      <c r="C1" s="192"/>
+      <c r="D1" s="192"/>
+      <c r="E1" s="192"/>
+      <c r="F1" s="192"/>
+      <c r="G1" s="192"/>
+      <c r="H1" s="192"/>
+      <c r="I1" s="192"/>
+      <c r="J1" s="192"/>
+      <c r="K1" s="192"/>
+      <c r="L1" s="192"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -26650,59 +26668,59 @@
       </c>
     </row>
     <row r="4" spans="1:18" s="59" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="201" t="s">
+      <c r="A4" s="186" t="s">
         <v>332</v>
       </c>
-      <c r="B4" s="202"/>
-      <c r="C4" s="202"/>
-      <c r="D4" s="202"/>
-      <c r="E4" s="202"/>
-      <c r="F4" s="202"/>
-      <c r="G4" s="202"/>
-      <c r="H4" s="202"/>
-      <c r="I4" s="202"/>
-      <c r="J4" s="202"/>
-      <c r="K4" s="202"/>
-      <c r="L4" s="203"/>
-      <c r="N4" s="200" t="s">
+      <c r="B4" s="187"/>
+      <c r="C4" s="187"/>
+      <c r="D4" s="187"/>
+      <c r="E4" s="187"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="187"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="188"/>
+      <c r="N4" s="185" t="s">
         <v>196</v>
       </c>
-      <c r="O4" s="200"/>
-      <c r="P4" s="200"/>
-      <c r="Q4" s="200"/>
-      <c r="R4" s="200"/>
+      <c r="O4" s="185"/>
+      <c r="P4" s="185"/>
+      <c r="Q4" s="185"/>
+      <c r="R4" s="185"/>
     </row>
     <row r="5" spans="1:18" s="94" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="201" t="s">
+      <c r="A5" s="186" t="s">
         <v>344</v>
       </c>
-      <c r="B5" s="202"/>
-      <c r="C5" s="202"/>
-      <c r="D5" s="202"/>
-      <c r="E5" s="202"/>
-      <c r="F5" s="202"/>
-      <c r="G5" s="202"/>
-      <c r="H5" s="202"/>
-      <c r="I5" s="202"/>
-      <c r="J5" s="202"/>
-      <c r="K5" s="202"/>
-      <c r="L5" s="203"/>
+      <c r="B5" s="187"/>
+      <c r="C5" s="187"/>
+      <c r="D5" s="187"/>
+      <c r="E5" s="187"/>
+      <c r="F5" s="187"/>
+      <c r="G5" s="187"/>
+      <c r="H5" s="187"/>
+      <c r="I5" s="187"/>
+      <c r="J5" s="187"/>
+      <c r="K5" s="187"/>
+      <c r="L5" s="188"/>
     </row>
     <row r="6" spans="1:18" s="94" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="204" t="s">
+      <c r="A6" s="189" t="s">
         <v>340</v>
       </c>
-      <c r="B6" s="205"/>
-      <c r="C6" s="205"/>
-      <c r="D6" s="205"/>
-      <c r="E6" s="205"/>
-      <c r="F6" s="205"/>
-      <c r="G6" s="205"/>
-      <c r="H6" s="205"/>
-      <c r="I6" s="205"/>
-      <c r="J6" s="205"/>
-      <c r="K6" s="205"/>
-      <c r="L6" s="206"/>
+      <c r="B6" s="190"/>
+      <c r="C6" s="190"/>
+      <c r="D6" s="190"/>
+      <c r="E6" s="190"/>
+      <c r="F6" s="190"/>
+      <c r="G6" s="190"/>
+      <c r="H6" s="190"/>
+      <c r="I6" s="190"/>
+      <c r="J6" s="190"/>
+      <c r="K6" s="190"/>
+      <c r="L6" s="191"/>
       <c r="N6" s="180" t="s">
         <v>347</v>
       </c>
@@ -26722,106 +26740,106 @@
       <c r="L7" s="125"/>
     </row>
     <row r="8" spans="1:18" s="94" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="195" t="s">
+      <c r="A8" s="203" t="s">
         <v>264</v>
       </c>
-      <c r="B8" s="196"/>
-      <c r="C8" s="196"/>
-      <c r="D8" s="196"/>
-      <c r="E8" s="196"/>
-      <c r="F8" s="196"/>
-      <c r="G8" s="196"/>
-      <c r="H8" s="196"/>
-      <c r="I8" s="196"/>
-      <c r="J8" s="196"/>
-      <c r="K8" s="196"/>
-      <c r="L8" s="197"/>
+      <c r="B8" s="204"/>
+      <c r="C8" s="204"/>
+      <c r="D8" s="204"/>
+      <c r="E8" s="204"/>
+      <c r="F8" s="204"/>
+      <c r="G8" s="204"/>
+      <c r="H8" s="204"/>
+      <c r="I8" s="204"/>
+      <c r="J8" s="204"/>
+      <c r="K8" s="204"/>
+      <c r="L8" s="205"/>
       <c r="N8" s="1" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="9" spans="1:18" s="94" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="192" t="s">
+      <c r="A9" s="200" t="s">
         <v>346</v>
       </c>
-      <c r="B9" s="193"/>
-      <c r="C9" s="193"/>
-      <c r="D9" s="193"/>
-      <c r="E9" s="193"/>
-      <c r="F9" s="193"/>
-      <c r="G9" s="193"/>
-      <c r="H9" s="193"/>
-      <c r="I9" s="193"/>
-      <c r="J9" s="193"/>
-      <c r="K9" s="193"/>
-      <c r="L9" s="194"/>
+      <c r="B9" s="201"/>
+      <c r="C9" s="201"/>
+      <c r="D9" s="201"/>
+      <c r="E9" s="201"/>
+      <c r="F9" s="201"/>
+      <c r="G9" s="201"/>
+      <c r="H9" s="201"/>
+      <c r="I9" s="201"/>
+      <c r="J9" s="201"/>
+      <c r="K9" s="201"/>
+      <c r="L9" s="202"/>
       <c r="N9" s="117" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:18" s="94" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="198" t="s">
+      <c r="A10" s="206" t="s">
         <v>265</v>
       </c>
-      <c r="B10" s="193"/>
-      <c r="C10" s="193"/>
-      <c r="D10" s="193"/>
-      <c r="E10" s="193"/>
-      <c r="F10" s="193"/>
-      <c r="G10" s="193"/>
-      <c r="H10" s="193"/>
-      <c r="I10" s="193"/>
-      <c r="J10" s="193"/>
-      <c r="K10" s="193"/>
-      <c r="L10" s="194"/>
+      <c r="B10" s="201"/>
+      <c r="C10" s="201"/>
+      <c r="D10" s="201"/>
+      <c r="E10" s="201"/>
+      <c r="F10" s="201"/>
+      <c r="G10" s="201"/>
+      <c r="H10" s="201"/>
+      <c r="I10" s="201"/>
+      <c r="J10" s="201"/>
+      <c r="K10" s="201"/>
+      <c r="L10" s="202"/>
     </row>
     <row r="11" spans="1:18" s="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="199" t="s">
+      <c r="A11" s="207" t="s">
         <v>262</v>
       </c>
-      <c r="B11" s="193"/>
-      <c r="C11" s="193"/>
-      <c r="D11" s="193"/>
-      <c r="E11" s="193"/>
-      <c r="F11" s="193"/>
-      <c r="G11" s="193"/>
-      <c r="H11" s="193"/>
-      <c r="I11" s="193"/>
-      <c r="J11" s="193"/>
-      <c r="K11" s="193"/>
-      <c r="L11" s="194"/>
+      <c r="B11" s="201"/>
+      <c r="C11" s="201"/>
+      <c r="D11" s="201"/>
+      <c r="E11" s="201"/>
+      <c r="F11" s="201"/>
+      <c r="G11" s="201"/>
+      <c r="H11" s="201"/>
+      <c r="I11" s="201"/>
+      <c r="J11" s="201"/>
+      <c r="K11" s="201"/>
+      <c r="L11" s="202"/>
     </row>
     <row r="12" spans="1:18" s="65" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="186" t="s">
+      <c r="A12" s="194" t="s">
         <v>266</v>
       </c>
-      <c r="B12" s="187"/>
-      <c r="C12" s="187"/>
-      <c r="D12" s="187"/>
-      <c r="E12" s="187"/>
-      <c r="F12" s="187"/>
-      <c r="G12" s="187"/>
-      <c r="H12" s="187"/>
-      <c r="I12" s="187"/>
-      <c r="J12" s="187"/>
-      <c r="K12" s="187"/>
-      <c r="L12" s="188"/>
+      <c r="B12" s="195"/>
+      <c r="C12" s="195"/>
+      <c r="D12" s="195"/>
+      <c r="E12" s="195"/>
+      <c r="F12" s="195"/>
+      <c r="G12" s="195"/>
+      <c r="H12" s="195"/>
+      <c r="I12" s="195"/>
+      <c r="J12" s="195"/>
+      <c r="K12" s="195"/>
+      <c r="L12" s="196"/>
     </row>
     <row r="13" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="189" t="s">
+      <c r="A13" s="197" t="s">
         <v>341</v>
       </c>
-      <c r="B13" s="190"/>
-      <c r="C13" s="190"/>
-      <c r="D13" s="190"/>
-      <c r="E13" s="190"/>
-      <c r="F13" s="190"/>
-      <c r="G13" s="190"/>
-      <c r="H13" s="190"/>
-      <c r="I13" s="190"/>
-      <c r="J13" s="190"/>
-      <c r="K13" s="190"/>
-      <c r="L13" s="191"/>
+      <c r="B13" s="198"/>
+      <c r="C13" s="198"/>
+      <c r="D13" s="198"/>
+      <c r="E13" s="198"/>
+      <c r="F13" s="198"/>
+      <c r="G13" s="198"/>
+      <c r="H13" s="198"/>
+      <c r="I13" s="198"/>
+      <c r="J13" s="198"/>
+      <c r="K13" s="198"/>
+      <c r="L13" s="199"/>
     </row>
     <row r="14" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="146"/>
@@ -26985,30 +27003,25 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="185" t="s">
+      <c r="A37" s="193" t="s">
         <v>343</v>
       </c>
-      <c r="B37" s="185"/>
-      <c r="C37" s="185"/>
-      <c r="D37" s="185"/>
-      <c r="E37" s="185"/>
-      <c r="F37" s="185"/>
-      <c r="G37" s="185"/>
-      <c r="H37" s="185"/>
-      <c r="I37" s="185"/>
-      <c r="J37" s="185"/>
-      <c r="K37" s="185"/>
-      <c r="L37" s="185"/>
+      <c r="B37" s="193"/>
+      <c r="C37" s="193"/>
+      <c r="D37" s="193"/>
+      <c r="E37" s="193"/>
+      <c r="F37" s="193"/>
+      <c r="G37" s="193"/>
+      <c r="H37" s="193"/>
+      <c r="I37" s="193"/>
+      <c r="J37" s="193"/>
+      <c r="K37" s="193"/>
+      <c r="L37" s="193"/>
     </row>
     <row r="42" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A1:L1"/>
     <mergeCell ref="A37:L37"/>
     <mergeCell ref="A12:L12"/>
     <mergeCell ref="A13:L13"/>
@@ -27016,6 +27029,11 @@
     <mergeCell ref="A8:L8"/>
     <mergeCell ref="A10:L10"/>
     <mergeCell ref="A11:L11"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A30" r:id="rId1" xr:uid="{6B934EC2-E381-41EE-938C-08FAF5E51BBE}"/>
@@ -42080,10 +42098,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BF02C3-B992-44C7-A79C-D1E41573911A}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42139,59 +42157,59 @@
       <c r="I2" s="41"/>
       <c r="J2" s="42"/>
     </row>
-    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="62">
         <v>44581</v>
       </c>
       <c r="B3" s="168" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="C3" s="61" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="D3" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E3" s="60" t="s">
-        <v>362</v>
-      </c>
-      <c r="F3" s="62" t="s">
-        <v>363</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F3" s="62"/>
       <c r="H3" s="41"/>
       <c r="I3" s="41"/>
       <c r="J3" s="42"/>
     </row>
     <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="62">
-        <v>44532</v>
+        <v>44581</v>
       </c>
       <c r="B4" s="168" t="s">
-        <v>339</v>
+        <v>360</v>
       </c>
       <c r="C4" s="61" t="s">
-        <v>348</v>
+        <v>361</v>
       </c>
       <c r="D4" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="62"/>
+        <v>362</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>363</v>
+      </c>
       <c r="H4" s="41"/>
       <c r="I4" s="41"/>
       <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="62">
-        <v>44501</v>
+        <v>44532</v>
       </c>
       <c r="B5" s="168" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>95</v>
@@ -42206,13 +42224,13 @@
     </row>
     <row r="6" spans="1:10" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="62">
-        <v>44500</v>
+        <v>44501</v>
       </c>
       <c r="B6" s="168" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C6" s="61" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D6" s="60" t="s">
         <v>95</v>
@@ -42229,21 +42247,21 @@
       </c>
       <c r="J6" s="42"/>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="62">
-        <v>44496</v>
+        <v>44500</v>
       </c>
       <c r="B7" s="168" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="D7" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E7" s="60" t="s">
-        <v>321</v>
+        <v>95</v>
       </c>
       <c r="F7" s="62"/>
       <c r="H7" s="41" t="s">
@@ -42256,25 +42274,23 @@
         <v>44482</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="62">
         <v>44496</v>
       </c>
       <c r="B8" s="168" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C8" s="61" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D8" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E8" s="60" t="s">
-        <v>349</v>
-      </c>
-      <c r="F8" s="62">
-        <v>44495</v>
-      </c>
+        <v>321</v>
+      </c>
+      <c r="F8" s="62"/>
       <c r="H8" s="41" t="s">
         <v>323</v>
       </c>
@@ -42283,21 +42299,25 @@
       </c>
       <c r="J8" s="43"/>
     </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="62">
-        <v>44480</v>
+        <v>44496</v>
       </c>
       <c r="B9" s="168" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="C9" s="61" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="D9" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="60"/>
-      <c r="F9" s="62"/>
+      <c r="E9" s="60" t="s">
+        <v>349</v>
+      </c>
+      <c r="F9" s="62">
+        <v>44495</v>
+      </c>
       <c r="H9" s="41" t="s">
         <v>159</v>
       </c>
@@ -42313,17 +42333,15 @@
         <v>44480</v>
       </c>
       <c r="B10" s="168" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C10" s="61" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="D10" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="60" t="s">
-        <v>95</v>
-      </c>
+      <c r="E10" s="60"/>
       <c r="F10" s="62"/>
       <c r="H10" s="41" t="s">
         <v>206</v>
@@ -42340,20 +42358,18 @@
         <v>44480</v>
       </c>
       <c r="B11" s="168" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C11" s="61" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D11" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E11" s="60" t="s">
-        <v>270</v>
-      </c>
-      <c r="F11" s="62" t="s">
-        <v>271</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F11" s="62"/>
       <c r="H11" s="41" t="s">
         <v>157</v>
       </c>
@@ -42366,21 +42382,23 @@
     </row>
     <row r="12" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="62">
-        <v>44474</v>
-      </c>
-      <c r="B12" s="60">
-        <v>3.7</v>
+        <v>44480</v>
+      </c>
+      <c r="B12" s="168" t="s">
+        <v>318</v>
       </c>
       <c r="C12" s="61" t="s">
-        <v>253</v>
+        <v>315</v>
       </c>
       <c r="D12" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E12" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" s="62"/>
+        <v>270</v>
+      </c>
+      <c r="F12" s="62" t="s">
+        <v>271</v>
+      </c>
       <c r="H12" s="41" t="s">
         <v>158</v>
       </c>
@@ -42393,57 +42411,57 @@
     </row>
     <row r="13" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="62">
-        <v>44463</v>
-      </c>
-      <c r="B13" s="60" t="s">
-        <v>334</v>
+        <v>44474</v>
+      </c>
+      <c r="B13" s="60">
+        <v>3.7</v>
       </c>
       <c r="C13" s="61" t="s">
-        <v>235</v>
+        <v>253</v>
       </c>
       <c r="D13" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E13" s="60" t="s">
-        <v>350</v>
-      </c>
-      <c r="F13" s="62">
-        <v>44432</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F13" s="62"/>
       <c r="H13" s="41"/>
       <c r="I13" s="41"/>
       <c r="J13" s="42"/>
     </row>
-    <row r="14" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="62">
-        <v>44459</v>
+        <v>44463</v>
       </c>
       <c r="B14" s="60" t="s">
-        <v>217</v>
+        <v>334</v>
       </c>
       <c r="C14" s="61" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
       <c r="D14" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E14" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="F14" s="62"/>
+        <v>350</v>
+      </c>
+      <c r="F14" s="62">
+        <v>44432</v>
+      </c>
       <c r="H14" s="41"/>
       <c r="I14" s="41"/>
       <c r="J14" s="42"/>
     </row>
-    <row r="15" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="62">
         <v>44459</v>
       </c>
-      <c r="B15" s="60">
-        <v>3.6</v>
+      <c r="B15" s="60" t="s">
+        <v>217</v>
       </c>
       <c r="C15" s="61" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D15" s="60" t="s">
         <v>95</v>
@@ -42456,15 +42474,15 @@
       <c r="I15" s="41"/>
       <c r="J15" s="42"/>
     </row>
-    <row r="16" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="62">
-        <v>44432</v>
+        <v>44459</v>
       </c>
       <c r="B16" s="60">
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="C16" s="61" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="D16" s="60" t="s">
         <v>95</v>
@@ -42472,14 +42490,12 @@
       <c r="E16" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="62">
-        <v>44424</v>
-      </c>
+      <c r="F16" s="62"/>
       <c r="H16" s="41"/>
       <c r="I16" s="41"/>
       <c r="J16" s="42"/>
     </row>
-    <row r="17" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="62">
         <v>44432</v>
       </c>
@@ -42487,19 +42503,19 @@
         <v>3.5</v>
       </c>
       <c r="C17" s="61" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D17" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E17" s="60" t="s">
-        <v>351</v>
+        <v>95</v>
       </c>
       <c r="F17" s="62">
         <v>44424</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="62">
         <v>44432</v>
       </c>
@@ -42507,101 +42523,101 @@
         <v>3.5</v>
       </c>
       <c r="C18" s="61" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
       <c r="D18" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="E18" s="60"/>
-      <c r="F18" s="62"/>
-    </row>
-    <row r="19" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E18" s="60" t="s">
+        <v>351</v>
+      </c>
+      <c r="F18" s="62">
+        <v>44424</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="62">
-        <v>44423</v>
-      </c>
-      <c r="B19" s="60" t="s">
-        <v>203</v>
+        <v>44432</v>
+      </c>
+      <c r="B19" s="60">
+        <v>3.5</v>
       </c>
       <c r="C19" s="61" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D19" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="E19" s="60" t="s">
-        <v>95</v>
-      </c>
+      <c r="E19" s="60"/>
       <c r="F19" s="62"/>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="62">
-        <v>44405</v>
+        <v>44423</v>
       </c>
       <c r="B20" s="60" t="s">
-        <v>200</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>202</v>
+        <v>203</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>204</v>
       </c>
       <c r="D20" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E20" s="60" t="s">
-        <v>352</v>
-      </c>
-      <c r="F20" s="62">
-        <v>44405</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F20" s="62"/>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="62">
         <v>44405</v>
       </c>
       <c r="B21" s="60" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" s="61" t="s">
-        <v>199</v>
+        <v>200</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>202</v>
       </c>
       <c r="D21" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E21" s="60" t="s">
-        <v>95</v>
+        <v>352</v>
       </c>
       <c r="F21" s="62">
         <v>44405</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="62">
         <v>44405</v>
       </c>
       <c r="B22" s="60" t="s">
-        <v>183</v>
+        <v>198</v>
       </c>
       <c r="C22" s="61" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D22" s="60" t="s">
         <v>95</v>
       </c>
       <c r="E22" s="60" t="s">
-        <v>352</v>
+        <v>95</v>
       </c>
       <c r="F22" s="62">
-        <v>44391</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="60" t="s">
-        <v>180</v>
+        <v>44405</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A23" s="62">
+        <v>44405</v>
       </c>
       <c r="B23" s="60" t="s">
-        <v>179</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>181</v>
+        <v>183</v>
+      </c>
+      <c r="C23" s="61" t="s">
+        <v>197</v>
       </c>
       <c r="D23" s="60" t="s">
         <v>95</v>
@@ -42613,7 +42629,7 @@
         <v>44391</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="60" t="s">
         <v>180</v>
       </c>
@@ -42621,7 +42637,7 @@
         <v>179</v>
       </c>
       <c r="C24" s="41" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="D24" s="60" t="s">
         <v>95</v>
@@ -42633,15 +42649,15 @@
         <v>44391</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A25" s="62">
-        <v>44403</v>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="60" t="s">
+        <v>180</v>
       </c>
       <c r="B25" s="60" t="s">
-        <v>160</v>
-      </c>
-      <c r="C25" s="61" t="s">
-        <v>161</v>
+        <v>179</v>
+      </c>
+      <c r="C25" s="41" t="s">
+        <v>156</v>
       </c>
       <c r="D25" s="60" t="s">
         <v>95</v>
@@ -42653,76 +42669,75 @@
         <v>44391</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="43">
-        <v>44389</v>
-      </c>
-      <c r="B26" s="42" t="s">
-        <v>152</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>153</v>
-      </c>
-      <c r="D26" s="44" t="s">
+    <row r="26" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A26" s="62">
+        <v>44403</v>
+      </c>
+      <c r="B26" s="60" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="E26" s="44" t="s">
-        <v>95</v>
-      </c>
-      <c r="F26" s="43">
-        <v>44389</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="E26" s="60" t="s">
+        <v>352</v>
+      </c>
+      <c r="F26" s="62">
+        <v>44391</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="43">
         <v>44389</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C27" s="41" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D27" s="44" t="s">
         <v>95</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>155</v>
+        <v>95</v>
       </c>
       <c r="F27" s="43">
-        <v>44385</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>44389</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="43">
-        <v>44385</v>
+        <v>44389</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="C28" s="41" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="D28" s="44" t="s">
         <v>95</v>
       </c>
       <c r="E28" s="44" t="s">
-        <v>95</v>
+        <v>155</v>
       </c>
       <c r="F28" s="43">
-        <f>A28</f>
         <v>44385</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="43">
-        <v>44384</v>
+        <v>44385</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C29" s="41" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D29" s="44" t="s">
         <v>95</v>
@@ -42731,18 +42746,19 @@
         <v>95</v>
       </c>
       <c r="F29" s="43">
-        <v>44384</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <f>A29</f>
+        <v>44385</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="43">
         <v>44384</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D30" s="44" t="s">
         <v>95</v>
@@ -42754,15 +42770,15 @@
         <v>44384</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="43">
-        <v>44378</v>
+        <v>44384</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C31" s="41" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="D31" s="44" t="s">
         <v>95</v>
@@ -42771,18 +42787,18 @@
         <v>95</v>
       </c>
       <c r="F31" s="43">
+        <v>44384</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="43">
         <v>44378</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="43">
-        <v>44377</v>
-      </c>
       <c r="B32" s="42" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D32" s="44" t="s">
         <v>95</v>
@@ -42791,38 +42807,38 @@
         <v>95</v>
       </c>
       <c r="F32" s="43">
-        <v>44377</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>44378</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="43">
         <v>44377</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="D33" s="44" t="s">
         <v>95</v>
       </c>
       <c r="E33" s="44" t="s">
-        <v>353</v>
+        <v>95</v>
       </c>
       <c r="F33" s="43">
-        <v>44372</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>44377</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="43">
         <v>44377</v>
       </c>
-      <c r="B34" s="42">
-        <v>3.3</v>
+      <c r="B34" s="42" t="s">
+        <v>115</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D34" s="44" t="s">
         <v>95</v>
@@ -42834,35 +42850,35 @@
         <v>44372</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="43">
         <v>44377</v>
       </c>
-      <c r="B35" s="42" t="s">
-        <v>112</v>
+      <c r="B35" s="42">
+        <v>3.3</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D35" s="44" t="s">
         <v>95</v>
       </c>
       <c r="E35" s="44" t="s">
-        <v>95</v>
+        <v>353</v>
       </c>
       <c r="F35" s="43">
+        <v>44372</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="43">
         <v>44377</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A36" s="43">
-        <v>44367</v>
-      </c>
-      <c r="B36" s="42">
-        <v>3.2</v>
+      <c r="B36" s="42" t="s">
+        <v>112</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D36" s="44" t="s">
         <v>95</v>
@@ -42871,18 +42887,18 @@
         <v>95</v>
       </c>
       <c r="F36" s="43">
+        <v>44377</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A37" s="43">
         <v>44367</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="43">
-        <v>44331</v>
-      </c>
       <c r="B37" s="42">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D37" s="44" t="s">
         <v>95</v>
@@ -42891,86 +42907,106 @@
         <v>95</v>
       </c>
       <c r="F37" s="43">
+        <v>44367</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="43">
         <v>44331</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A38" s="43">
-        <v>44319</v>
-      </c>
       <c r="B38" s="42">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D38" s="44" t="s">
         <v>95</v>
       </c>
       <c r="E38" s="44" t="s">
-        <v>354</v>
+        <v>95</v>
       </c>
       <c r="F38" s="43">
-        <v>44315</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>44331</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A39" s="43">
-        <v>44307</v>
+        <v>44319</v>
       </c>
       <c r="B39" s="42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39" s="41" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D39" s="44" t="s">
         <v>95</v>
       </c>
       <c r="E39" s="44" t="s">
-        <v>155</v>
+        <v>354</v>
       </c>
       <c r="F39" s="43">
-        <v>44294</v>
+        <v>44315</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="43">
-        <v>44293</v>
-      </c>
-      <c r="B40" s="45">
-        <v>1</v>
+        <v>44307</v>
+      </c>
+      <c r="B40" s="42">
+        <v>2</v>
       </c>
       <c r="C40" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D40" s="44" t="s">
         <v>95</v>
       </c>
       <c r="E40" s="44" t="s">
-        <v>354</v>
+        <v>155</v>
       </c>
       <c r="F40" s="43">
-        <v>44291</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44294</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="43">
-        <v>44291</v>
+        <v>44293</v>
       </c>
       <c r="B41" s="45">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C41" s="41" t="s">
-        <v>333</v>
+        <v>106</v>
       </c>
       <c r="D41" s="44" t="s">
         <v>95</v>
       </c>
       <c r="E41" s="44" t="s">
+        <v>354</v>
+      </c>
+      <c r="F41" s="43">
+        <v>44291</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="43">
+        <v>44291</v>
+      </c>
+      <c r="B42" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="C42" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="D42" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="F41" s="43">
+      <c r="E42" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" s="43">
         <v>44285</v>
       </c>
     </row>
@@ -42983,7 +43019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -48437,10 +48473,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C26E2B-D89A-4E77-AA63-A653F9E68AE0}">
-  <dimension ref="A1:P144"/>
+  <dimension ref="A1:P142"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView topLeftCell="A78" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -48581,7 +48617,9 @@
       <c r="B8" s="183" t="s">
         <v>356</v>
       </c>
-      <c r="C8" s="217"/>
+      <c r="C8" s="222" t="s">
+        <v>357</v>
+      </c>
       <c r="D8" s="217"/>
       <c r="E8" s="217"/>
       <c r="F8" s="217"/>
@@ -48593,12 +48631,17 @@
         <f>IF(Master!A9="","",Master!A9)</f>
         <v>First Nations</v>
       </c>
-      <c r="B9" s="181"/>
-      <c r="C9" s="223"/>
-      <c r="D9" s="223"/>
-      <c r="E9" s="223"/>
-      <c r="F9" s="223"/>
-      <c r="G9" s="223"/>
+      <c r="B9" s="183" t="str">
+        <f>IF($A9&lt;&gt;"",B8,"")</f>
+        <v>Law</v>
+      </c>
+      <c r="C9" s="237" t="s">
+        <v>365</v>
+      </c>
+      <c r="D9" s="238"/>
+      <c r="E9" s="238"/>
+      <c r="F9" s="238"/>
+      <c r="G9" s="239"/>
       <c r="N9" s="160"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -50503,11 +50546,11 @@
         <v xml:space="preserve">   Enter withdraw [maf] within available water</v>
       </c>
       <c r="C65" s="104" t="str">
-        <f>IF(C$28&lt;&gt;"",IF(C64&gt;4.2,4.2,MAX(C64,0)),"")</f>
+        <f t="shared" ref="C65:G65" si="22">IF(C$28&lt;&gt;"",IF(C64&gt;4.2,4.2,MAX(C64,0)),"")</f>
         <v/>
       </c>
       <c r="D65" s="104" t="str">
-        <f t="shared" ref="D65:G65" si="22">IF(D$28&lt;&gt;"",IF(D64&gt;4.2,4.2,MAX(D64,0)),"")</f>
+        <f t="shared" si="22"/>
         <v/>
       </c>
       <c r="E65" s="104" t="str">
@@ -51534,11 +51577,26 @@
         <f>IF(A96="","",$A$65)</f>
         <v xml:space="preserve">   Enter withdraw [maf] within available water</v>
       </c>
-      <c r="C97" s="104"/>
-      <c r="D97" s="104"/>
-      <c r="E97" s="104"/>
-      <c r="F97" s="104"/>
-      <c r="G97" s="104"/>
+      <c r="C97" s="104" t="str">
+        <f>IF(OR(C$28="",$A97=""),"",C96)</f>
+        <v/>
+      </c>
+      <c r="D97" s="104" t="str">
+        <f t="shared" ref="D97:G97" si="37">IF(OR(D$28="",$A97=""),"",D96)</f>
+        <v/>
+      </c>
+      <c r="E97" s="104" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="F97" s="104" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="G97" s="104" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
       <c r="H97" s="104"/>
       <c r="I97" s="104"/>
       <c r="J97" s="104"/>
@@ -51558,39 +51616,39 @@
         <v/>
       </c>
       <c r="D98" s="47" t="str">
-        <f t="shared" ref="D98:L98" si="37">IF(OR(D$28="",$A98=""),"",D96-D97)</f>
+        <f t="shared" ref="D98:L98" si="38">IF(OR(D$28="",$A98=""),"",D96-D97)</f>
         <v/>
       </c>
       <c r="E98" s="47" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="F98" s="47" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="G98" s="47" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="H98" s="47" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="I98" s="47" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="J98" s="47" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="K98" s="47" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="L98" s="47" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v/>
       </c>
       <c r="N98" s="159" t="s">
@@ -51672,47 +51730,47 @@
         <v xml:space="preserve">   Net trade volume all players (should be zero)</v>
       </c>
       <c r="C103" s="48" t="str">
-        <f t="shared" ref="C103:M103" si="38">IF(OR(C$28="",$A103=""),"",C$116)</f>
+        <f t="shared" ref="C103:M103" si="39">IF(OR(C$28="",$A103=""),"",C$116)</f>
         <v/>
       </c>
       <c r="D103" s="48" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="E103" s="48" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="F103" s="48" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="G103" s="48" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="H103" s="48" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="I103" s="48" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="J103" s="48" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="K103" s="48" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="L103" s="48" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="M103" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v/>
       </c>
       <c r="N103" s="160"/>
@@ -51727,39 +51785,39 @@
         <v/>
       </c>
       <c r="D104" s="13" t="str">
-        <f t="shared" ref="D104:L104" si="39">IF(OR(D$28="",$A104=""),"",D38+D56-D48+D101)</f>
+        <f t="shared" ref="D104:L104" si="40">IF(OR(D$28="",$A104=""),"",D38+D56-D48+D101)</f>
         <v/>
       </c>
       <c r="E104" s="13" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="F104" s="13" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="G104" s="13" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="H104" s="13" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="I104" s="13" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="J104" s="13" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="K104" s="13" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="L104" s="13" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="N104" s="160"/>
@@ -51791,39 +51849,39 @@
         <v/>
       </c>
       <c r="D106" s="47" t="str">
-        <f t="shared" ref="D106:L106" si="40">IF(OR(D$28="",$A106=""),"",D104-D105)</f>
+        <f t="shared" ref="D106:L106" si="41">IF(OR(D$28="",$A106=""),"",D104-D105)</f>
         <v/>
       </c>
       <c r="E106" s="47" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="F106" s="47" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="G106" s="47" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="H106" s="47" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="I106" s="47" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="J106" s="47" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="K106" s="47" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="L106" s="47" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v/>
       </c>
       <c r="N106" s="160"/>
@@ -51864,48 +51922,48 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" t="str">
-        <f t="shared" ref="A110:A115" si="41">IF(A5="","","    "&amp;A5)</f>
+        <f t="shared" ref="A110:A115" si="42">IF(A5="","","    "&amp;A5)</f>
         <v xml:space="preserve">    Upper Basin</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="48" t="str">
-        <f t="shared" ref="C110:L115" ca="1" si="42">IF(OR(C$28="",$A110=""),"",OFFSET(C$61,8*(ROW(B110)-ROW(B$110)),0))</f>
+        <f t="shared" ref="C110:L115" ca="1" si="43">IF(OR(C$28="",$A110=""),"",OFFSET(C$61,8*(ROW(B110)-ROW(B$110)),0))</f>
         <v/>
       </c>
       <c r="D110" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="E110" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="F110" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="G110" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="H110" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="I110" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="J110" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="K110" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="L110" s="150" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="M110" s="151">
@@ -51916,260 +51974,260 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v xml:space="preserve">    Lower Basin</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="D111" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="E111" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="F111" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="G111" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="H111" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="I111" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="J111" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="K111" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="L111" s="150" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="M111" s="151">
-        <f t="shared" ref="M111:M115" ca="1" si="43">IF(OR($A111=""),"",SUM(C111:L111))</f>
+        <f t="shared" ref="M111:M115" ca="1" si="44">IF(OR($A111=""),"",SUM(C111:L111))</f>
         <v>0</v>
       </c>
       <c r="N111" s="164"/>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v xml:space="preserve">    Mexico</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="D112" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="E112" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="F112" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="G112" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="H112" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="I112" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="J112" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="K112" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="L112" s="150" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="M112" s="151">
-        <f t="shared" ca="1" si="43"/>
+        <f t="shared" ca="1" si="44"/>
         <v>0</v>
       </c>
       <c r="N112" s="164"/>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v xml:space="preserve">    Colorado River Delta</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="D113" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="E113" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="F113" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="G113" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="H113" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="I113" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="J113" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="K113" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="L113" s="150" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="M113" s="151">
-        <f t="shared" ca="1" si="43"/>
+        <f t="shared" ca="1" si="44"/>
         <v>0</v>
       </c>
       <c r="N113" s="164"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v xml:space="preserve">    First Nations</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="D114" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="E114" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="F114" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="G114" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="H114" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="I114" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="J114" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="K114" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="L114" s="150" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="M114" s="151">
-        <f t="shared" ca="1" si="43"/>
+        <f t="shared" ca="1" si="44"/>
         <v>0</v>
       </c>
       <c r="N114" s="164"/>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v xml:space="preserve">    Shared, Reserve</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="D115" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="E115" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="F115" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="G115" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="H115" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="I115" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="J115" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="K115" s="48" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="L115" s="150" t="str">
-        <f t="shared" ca="1" si="42"/>
+        <f t="shared" ca="1" si="43"/>
         <v/>
       </c>
       <c r="M115" s="151">
-        <f t="shared" ca="1" si="43"/>
+        <f t="shared" ca="1" si="44"/>
         <v>0</v>
       </c>
       <c r="N115" s="164"/>
@@ -52184,39 +52242,39 @@
         <v/>
       </c>
       <c r="D116" s="35" t="str">
-        <f t="shared" ref="D116:L116" si="44">IF(D$28&lt;&gt;"",SUM(D110:D115),"")</f>
+        <f t="shared" ref="D116:L116" si="45">IF(D$28&lt;&gt;"",SUM(D110:D115),"")</f>
         <v/>
       </c>
       <c r="E116" s="92" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="F116" s="35" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="G116" s="35" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="H116" s="35" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="I116" s="35" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="J116" s="35" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="K116" s="35" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="L116" s="35" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v/>
       </c>
       <c r="M116" s="22"/>
@@ -52245,43 +52303,43 @@
         <v xml:space="preserve">    Upper Basin - Consumptive Use and Headwaters Losses</v>
       </c>
       <c r="C118" s="48" t="str">
-        <f t="shared" ref="C118:L123" ca="1" si="45">IF(OR(C$28="",$A118=""),"",OFFSET(C$65,8*(ROW(B118)-ROW(B$118)),0))</f>
+        <f t="shared" ref="C118:L123" ca="1" si="46">IF(OR(C$28="",$A118=""),"",OFFSET(C$65,8*(ROW(B118)-ROW(B$118)),0))</f>
         <v/>
       </c>
       <c r="D118" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="E118" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="F118" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="G118" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="H118" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="I118" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="J118" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="K118" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="L118" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="N118" s="160"/>
@@ -52292,43 +52350,43 @@
         <v xml:space="preserve">    Lower Basin - Release from Mead</v>
       </c>
       <c r="C119" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="D119" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="E119" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="F119" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="G119" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="H119" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="I119" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="J119" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="K119" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="L119" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="N119" s="160"/>
@@ -52339,43 +52397,43 @@
         <v xml:space="preserve">    Mexico - Release from Mead</v>
       </c>
       <c r="C120" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="D120" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="E120" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="F120" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="G120" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="H120" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="I120" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="J120" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="K120" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="L120" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="N120" s="160"/>
@@ -52386,43 +52444,43 @@
         <v xml:space="preserve">    Colorado River Delta - Release from Mead</v>
       </c>
       <c r="C121" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="D121" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="E121" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="F121" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="G121" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="H121" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="I121" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="J121" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="K121" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="L121" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="N121" s="160"/>
@@ -52433,43 +52491,43 @@
         <v xml:space="preserve">    First Nations - Release from Mead</v>
       </c>
       <c r="C122" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="D122" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="E122" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="F122" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="G122" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="H122" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="I122" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="J122" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="K122" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="L122" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="N122" s="160"/>
@@ -52480,43 +52538,43 @@
         <v xml:space="preserve">    Shared, Reserve - Release from Mead</v>
       </c>
       <c r="C123" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="D123" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="E123" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="F123" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="G123" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="H123" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="I123" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="J123" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="K123" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="L123" s="48" t="str">
-        <f t="shared" ca="1" si="45"/>
+        <f t="shared" ca="1" si="46"/>
         <v/>
       </c>
       <c r="N123" s="160"/>
@@ -52539,282 +52597,282 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" t="str">
-        <f t="shared" ref="A125:A130" si="46">IF(A5="","","    "&amp;A5)</f>
+        <f t="shared" ref="A125:A130" si="47">IF(A5="","","    "&amp;A5)</f>
         <v xml:space="preserve">    Upper Basin</v>
       </c>
       <c r="C125" s="48" t="str">
-        <f t="shared" ref="C125:L130" ca="1" si="47">IF(OR(C$28="",$A125=""),"",OFFSET(C$66,8*(ROW(B125)-ROW(B$125)),0))</f>
+        <f t="shared" ref="C125:L130" ca="1" si="48">IF(OR(C$28="",$A125=""),"",OFFSET(C$66,8*(ROW(B125)-ROW(B$125)),0))</f>
         <v/>
       </c>
       <c r="D125" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="E125" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="F125" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="G125" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="H125" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="I125" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="J125" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="K125" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="L125" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="N125" s="160"/>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">    Lower Basin</v>
       </c>
       <c r="C126" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="D126" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="E126" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="F126" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="G126" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="H126" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="I126" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="J126" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="K126" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="L126" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="N126" s="160"/>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">    Mexico</v>
       </c>
       <c r="C127" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="D127" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="E127" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="F127" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="G127" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="H127" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="I127" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="J127" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="K127" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="L127" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="N127" s="160"/>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">    Colorado River Delta</v>
       </c>
       <c r="C128" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="D128" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="E128" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="F128" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="G128" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="H128" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="I128" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="J128" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="K128" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="L128" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="N128" s="160"/>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">    First Nations</v>
       </c>
       <c r="C129" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="D129" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="E129" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="F129" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="G129" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="H129" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="I129" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="J129" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="K129" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="L129" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="N129" s="160"/>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v xml:space="preserve">    Shared, Reserve</v>
       </c>
       <c r="C130" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="D130" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="E130" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="F130" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="G130" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="H130" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="I130" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="J130" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="K130" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="L130" s="48" t="str">
-        <f t="shared" ca="1" si="47"/>
+        <f t="shared" ca="1" si="48"/>
         <v/>
       </c>
       <c r="N130" s="160"/>
@@ -52829,39 +52887,39 @@
         <v/>
       </c>
       <c r="D131" s="13" t="str">
-        <f t="shared" ref="D131:L131" si="48">IF(D$28&lt;&gt;"",SUM(D125:D130),"")</f>
+        <f t="shared" ref="D131:L131" si="49">IF(D$28&lt;&gt;"",SUM(D125:D130),"")</f>
         <v/>
       </c>
       <c r="E131" s="13" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="F131" s="13" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="G131" s="13" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="H131" s="13" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="I131" s="13" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="J131" s="13" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="K131" s="13" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="L131" s="13" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v/>
       </c>
       <c r="N131" s="159" t="s">
@@ -52903,39 +52961,39 @@
         <v/>
       </c>
       <c r="D133" s="13" t="str">
-        <f t="shared" ref="D133:L133" si="49">IF(D28="","",D$132*D$131)</f>
+        <f t="shared" ref="D133:L133" si="50">IF(D28="","",D$132*D$131)</f>
         <v/>
       </c>
       <c r="E133" s="13" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="F133" s="13" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="G133" s="13" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="H133" s="13" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="I133" s="13" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="J133" s="13" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="K133" s="13" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="L133" s="13" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v/>
       </c>
       <c r="N133" s="159" t="s">
@@ -52952,39 +53010,39 @@
         <v/>
       </c>
       <c r="D134" s="13" t="str">
-        <f t="shared" ref="D134:L134" si="50">IF(D29="","",(1-D$132)*D$131)</f>
+        <f t="shared" ref="D134:L134" si="51">IF(D29="","",(1-D$132)*D$131)</f>
         <v/>
       </c>
       <c r="E134" s="13" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="F134" s="13" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="G134" s="13" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="H134" s="13" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="I134" s="13" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="J134" s="13" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="K134" s="13" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="L134" s="13" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v/>
       </c>
       <c r="N134" s="159" t="s">
@@ -53303,17 +53361,8 @@
         <v>308</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D144" s="15"/>
-    </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="A132:B132"/>
     <mergeCell ref="C8:G8"/>
@@ -53322,6 +53371,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <conditionalFormatting sqref="H73">
     <cfRule type="cellIs" dxfId="48" priority="63" operator="greaterThan">
@@ -53376,31 +53431,6 @@
   <conditionalFormatting sqref="C89:L89">
     <cfRule type="cellIs" dxfId="38" priority="53" operator="greaterThan">
       <formula>$C$88</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C97">
-    <cfRule type="cellIs" dxfId="37" priority="52" operator="greaterThan">
-      <formula>$C$96</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D97">
-    <cfRule type="cellIs" dxfId="36" priority="51" operator="greaterThan">
-      <formula>$D$96</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E97">
-    <cfRule type="cellIs" dxfId="35" priority="50" operator="greaterThan">
-      <formula>$E$96</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F97">
-    <cfRule type="cellIs" dxfId="34" priority="49" operator="greaterThan">
-      <formula>$F$96</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G97">
-    <cfRule type="cellIs" dxfId="33" priority="48" operator="greaterThan">
-      <formula>$G$96</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H97">
@@ -53747,7 +53777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF413BB-D622-46C1-9841-0489E9AA7BE8}">
   <dimension ref="G1:X1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="X34" sqref="X34"/>
     </sheetView>
   </sheetViews>

</xml_diff>